<commit_message>
cash purchases for projects
</commit_message>
<xml_diff>
--- a/public/uploads/media/default/sample_project_budgets.xlsx
+++ b/public/uploads/media/default/sample_project_budgets.xlsx
@@ -5,12 +5,12 @@
   <workbookPr codeName="ThisWorkbook"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\sahaf\Downloads\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\sahaf\Desktop\Mohamed\Sahafintech\ekstrabooks-v2.0\public\uploads\media\default\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C8CB9E2D-86E6-4EC4-AC81-6196B9C42DD7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CB7FD5CE-0100-4385-926C-73EAB84AE3BF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Project Budgets" sheetId="1" r:id="rId1"/>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="24" uniqueCount="24">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="19" uniqueCount="19">
   <si>
     <t>task_code</t>
   </si>
@@ -56,33 +56,6 @@
     <t>original_budgeted_amount</t>
   </si>
   <si>
-    <t>revised_budgeted_quantity</t>
-  </si>
-  <si>
-    <t>revised_budgeted_amount</t>
-  </si>
-  <si>
-    <t>revised_committed_quantity</t>
-  </si>
-  <si>
-    <t>revised_committed_amount</t>
-  </si>
-  <si>
-    <t>committed_open_quantity</t>
-  </si>
-  <si>
-    <t>committed_open_amount</t>
-  </si>
-  <si>
-    <t>committed_received_quantity</t>
-  </si>
-  <si>
-    <t>committed_invoiced_quantity</t>
-  </si>
-  <si>
-    <t>committed_invoiced_amount</t>
-  </si>
-  <si>
     <t>actual_quantity</t>
   </si>
   <si>
@@ -101,10 +74,22 @@
     <t>working on woods</t>
   </si>
   <si>
-    <t>Hours</t>
-  </si>
-  <si>
     <t>project_code</t>
+  </si>
+  <si>
+    <t>Piece</t>
+  </si>
+  <si>
+    <t>committed_budget_quantity</t>
+  </si>
+  <si>
+    <t>committed_budget_amount</t>
+  </si>
+  <si>
+    <t>received_budget_quantity</t>
+  </si>
+  <si>
+    <t>received_budget_amount</t>
   </si>
 </sst>
 </file>
@@ -456,36 +441,32 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:S2"/>
+  <dimension ref="A1:N2"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B5" sqref="B5"/>
+      <selection activeCell="L5" sqref="L5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultColWidth="12.7109375" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="12.6328125" bestFit="1" customWidth="1"/>
-    <col min="2" max="3" width="9.90625" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="16.1796875" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="5.81640625" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="9.1796875" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="26.453125" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="25.90625" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="26.08984375" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="25.54296875" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="27.26953125" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="26.7265625" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="25.453125" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="24.81640625" bestFit="1" customWidth="1"/>
-    <col min="15" max="16" width="28.453125" bestFit="1" customWidth="1"/>
-    <col min="17" max="17" width="27.90625" bestFit="1" customWidth="1"/>
-    <col min="18" max="18" width="15.1796875" bestFit="1" customWidth="1"/>
-    <col min="19" max="19" width="14.6328125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="13.140625" bestFit="1" customWidth="1"/>
+    <col min="2" max="3" width="10.42578125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="17.42578125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="6.140625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="9.42578125" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="27.140625" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="26.5703125" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="26.85546875" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="26.28515625" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="28" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="27.42578125" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="15.5703125" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="15" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:19" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:14" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
-        <v>23</v>
+        <v>13</v>
       </c>
       <c r="B1" s="1" t="s">
         <v>0</v>
@@ -509,54 +490,39 @@
         <v>6</v>
       </c>
       <c r="I1" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="J1" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="K1" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="L1" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="M1" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="J1" s="1" t="s">
+      <c r="N1" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="K1" s="1" t="s">
+    </row>
+    <row r="2" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
         <v>9</v>
       </c>
-      <c r="L1" s="1" t="s">
+      <c r="B2" t="s">
         <v>10</v>
       </c>
-      <c r="M1" s="1" t="s">
+      <c r="C2" t="s">
         <v>11</v>
       </c>
-      <c r="N1" s="1" t="s">
+      <c r="D2" t="s">
         <v>12</v>
       </c>
-      <c r="O1" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="P1" s="1" t="s">
+      <c r="E2" t="s">
         <v>14</v>
-      </c>
-      <c r="Q1" s="1" t="s">
-        <v>15</v>
-      </c>
-      <c r="R1" s="1" t="s">
-        <v>16</v>
-      </c>
-      <c r="S1" s="1" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="2" spans="1:19" x14ac:dyDescent="0.35">
-      <c r="A2" t="s">
-        <v>18</v>
-      </c>
-      <c r="B2" t="s">
-        <v>19</v>
-      </c>
-      <c r="C2" t="s">
-        <v>20</v>
-      </c>
-      <c r="D2" t="s">
-        <v>21</v>
-      </c>
-      <c r="E2" t="s">
-        <v>22</v>
       </c>
       <c r="F2">
         <v>16</v>
@@ -583,21 +549,6 @@
         <v>0</v>
       </c>
       <c r="N2">
-        <v>0</v>
-      </c>
-      <c r="O2">
-        <v>0</v>
-      </c>
-      <c r="P2">
-        <v>0</v>
-      </c>
-      <c r="Q2">
-        <v>0</v>
-      </c>
-      <c r="R2">
-        <v>0</v>
-      </c>
-      <c r="S2">
         <v>0</v>
       </c>
     </row>

</xml_diff>

<commit_message>
i made sure to right the sample excel headers to match the database
</commit_message>
<xml_diff>
--- a/public/uploads/media/default/sample_project_budgets.xlsx
+++ b/public/uploads/media/default/sample_project_budgets.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="28730"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="28827"/>
   <workbookPr codeName="ThisWorkbook"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\sahaf\Desktop\Mohamed\Sahafintech\ekstrabooks-v2.0\public\uploads\media\default\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CB7FD5CE-0100-4385-926C-73EAB84AE3BF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2A6E6877-36AE-4ECD-AF02-A27CAD6673DA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -56,12 +56,6 @@
     <t>original_budgeted_amount</t>
   </si>
   <si>
-    <t>actual_quantity</t>
-  </si>
-  <si>
-    <t>actual_amount</t>
-  </si>
-  <si>
     <t>JAH66273</t>
   </si>
   <si>
@@ -90,6 +84,12 @@
   </si>
   <si>
     <t>received_budget_amount</t>
+  </si>
+  <si>
+    <t>actual_budget_quantity</t>
+  </si>
+  <si>
+    <t>actual_budget_amount</t>
   </si>
 </sst>
 </file>
@@ -444,7 +444,7 @@
   <dimension ref="A1:N2"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="L5" sqref="L5"/>
+      <selection activeCell="N1" sqref="N1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.7109375" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -466,7 +466,7 @@
   <sheetData>
     <row r="1" spans="1:14" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="B1" s="1" t="s">
         <v>0</v>
@@ -490,39 +490,39 @@
         <v>6</v>
       </c>
       <c r="I1" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="J1" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="K1" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="J1" s="1" t="s">
+      <c r="L1" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="K1" s="1" t="s">
+      <c r="M1" s="1" t="s">
         <v>17</v>
       </c>
-      <c r="L1" s="1" t="s">
+      <c r="N1" s="1" t="s">
         <v>18</v>
-      </c>
-      <c r="M1" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="N1" s="1" t="s">
-        <v>8</v>
       </c>
     </row>
     <row r="2" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
+        <v>7</v>
+      </c>
+      <c r="B2" t="s">
+        <v>8</v>
+      </c>
+      <c r="C2" t="s">
         <v>9</v>
       </c>
-      <c r="B2" t="s">
+      <c r="D2" t="s">
         <v>10</v>
       </c>
-      <c r="C2" t="s">
-        <v>11</v>
-      </c>
-      <c r="D2" t="s">
+      <c r="E2" t="s">
         <v>12</v>
-      </c>
-      <c r="E2" t="s">
-        <v>14</v>
       </c>
       <c r="F2">
         <v>16</v>

</xml_diff>